<commit_message>
made test/new.py repeat function consistent with original
</commit_message>
<xml_diff>
--- a/normal_group.xlsx
+++ b/normal_group.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dyaqub/git/kobo-transfer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{563D90AB-0402-1F49-B914-69F54BBDD4FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C7322A-DFAF-6549-8521-9ECA804424B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="24840" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="normal group test" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>start</t>
   </si>
@@ -46,9 +46,6 @@
     <t>_id</t>
   </si>
   <si>
-    <t>_uuid</t>
-  </si>
-  <si>
     <t>_submission_time</t>
   </si>
   <si>
@@ -82,9 +79,6 @@
     <t>13:30:00.000+07:00</t>
   </si>
   <si>
-    <t>56ea0f6b-358a-4605-9452-5cf792a7e257</t>
-  </si>
-  <si>
     <t>submitted_via_web</t>
   </si>
   <si>
@@ -100,13 +94,7 @@
     <t>01:30:00.000+07:00</t>
   </si>
   <si>
-    <t>1c65fb96-b454-4b78-a5b4-8e84cf29b72b</t>
-  </si>
-  <si>
     <t>01:15:00.000+07:00</t>
-  </si>
-  <si>
-    <t>d432048f-12a1-43ee-bf75-ab7bdc52756e</t>
   </si>
   <si>
     <t>test numba 3 (changed)</t>
@@ -456,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -467,7 +455,7 @@
     <col min="6" max="6" width="41.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -516,11 +504,8 @@
       <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>45341.553854502323</v>
       </c>
@@ -528,40 +513,37 @@
         <v>45341.553945034721</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2">
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1">
         <v>45336</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H2">
         <v>313801375</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="1">
+        <v>45341.262291666673</v>
+      </c>
+      <c r="L2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="1">
-        <v>45341.262291666673</v>
-      </c>
-      <c r="M2" t="s">
-        <v>21</v>
-      </c>
-      <c r="O2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q2">
+      <c r="P2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>45341.553945243053</v>
       </c>
@@ -569,37 +551,34 @@
         <v>45341.554054583343</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D3">
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H3">
         <v>313801398</v>
       </c>
-      <c r="I3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" s="1">
+      <c r="I3" s="1">
         <v>45341.262395833342</v>
       </c>
-      <c r="M3" t="s">
-        <v>21</v>
-      </c>
-      <c r="O3" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q3">
+      <c r="L3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>45341.554054849526</v>
       </c>
@@ -610,30 +589,27 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F4" s="2">
         <v>45575</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H4">
         <v>313801475</v>
       </c>
-      <c r="I4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" s="1">
+      <c r="I4" s="1">
         <v>45341.262696759259</v>
       </c>
-      <c r="M4" t="s">
-        <v>21</v>
-      </c>
-      <c r="O4" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q4">
+      <c r="L4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P4">
         <v>3</v>
       </c>
     </row>

</xml_diff>